<commit_message>
DiSCoVER ran on all PDXs, reports created
</commit_message>
<xml_diff>
--- a/Notebooks/results/cell_lines_median_ranking.xlsx
+++ b/Notebooks/results/cell_lines_median_ranking.xlsx
@@ -916,7 +916,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -924,6 +924,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF079E25"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF44D4F4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -18785,6 +18795,33 @@
     <cfRule type="expression" dxfId="0" priority="7">
       <formula>INDIRECT("A"&amp;ROW())="gliosarcoma"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>INDIRECT("A"&amp;ROW())="Amelanotic melanoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>INDIRECT("A"&amp;ROW())="Hepatoblastoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>INDIRECT("A"&amp;ROW())="Rectosigmoid adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>INDIRECT("A"&amp;ROW())="Invasive ductal carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinomaype"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>INDIRECT("A"&amp;ROW())="vertebra"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28620,6 +28657,33 @@
     <cfRule type="expression" dxfId="0" priority="7">
       <formula>INDIRECT("A"&amp;ROW())="gliosarcoma"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>INDIRECT("A"&amp;ROW())="Amelanotic melanoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>INDIRECT("A"&amp;ROW())="Hepatoblastoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>INDIRECT("A"&amp;ROW())="Rectosigmoid adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>INDIRECT("A"&amp;ROW())="Invasive ductal carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinomaype"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>INDIRECT("A"&amp;ROW())="vertebra"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33811,6 +33875,33 @@
     <cfRule type="expression" dxfId="0" priority="7">
       <formula>INDIRECT("A"&amp;ROW())="gliosarcoma"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>INDIRECT("A"&amp;ROW())="Amelanotic melanoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>INDIRECT("A"&amp;ROW())="Hepatoblastoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>INDIRECT("A"&amp;ROW())="Rectosigmoid adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>INDIRECT("A"&amp;ROW())="Invasive ductal carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinomaype"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>INDIRECT("A"&amp;ROW())="vertebra"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40550,6 +40641,33 @@
     <cfRule type="expression" dxfId="0" priority="7">
       <formula>INDIRECT("A"&amp;ROW())="gliosarcoma"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>INDIRECT("A"&amp;ROW())="Amelanotic melanoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>INDIRECT("A"&amp;ROW())="Hepatoblastoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>INDIRECT("A"&amp;ROW())="Rectosigmoid adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>INDIRECT("A"&amp;ROW())="Invasive ductal carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinomaype"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>INDIRECT("A"&amp;ROW())="vertebra"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44967,6 +45085,33 @@
     <cfRule type="expression" dxfId="0" priority="7">
       <formula>INDIRECT("A"&amp;ROW())="gliosarcoma"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>INDIRECT("A"&amp;ROW())="Amelanotic melanoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>INDIRECT("A"&amp;ROW())="Lung adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>INDIRECT("A"&amp;ROW())="Hepatoblastoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>INDIRECT("A"&amp;ROW())="Rectosigmoid adenocarcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>INDIRECT("A"&amp;ROW())="Invasive ductal carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinoma"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="15">
+      <formula>INDIRECT("A"&amp;ROW())="Prostate carcinomaype"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>INDIRECT("A"&amp;ROW())="vertebra"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>